<commit_message>
qu'est ce qu'on a appris ce jour (live coding & algo)
</commit_message>
<xml_diff>
--- a/Journal De Bord YouCode 2021.xlsx
+++ b/Journal De Bord YouCode 2021.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>QU'EST-CE QU'ON A FAIS ?</t>
   </si>
@@ -160,12 +160,129 @@
   <si>
     <t>LE 15/11/2021</t>
   </si>
+  <si>
+    <t>We did a live coding about the conditions in C language and a presentation on the algorithm;</t>
+  </si>
+  <si>
+    <t>to program own programs and respect programming standards and not forget the complexity of a program</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Regarding live coding, we have studied the role of:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Break:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> which allows the exit of a block of code 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>return 0</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">: quit a function.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>continue</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">: to continue a block of code (unlike Break)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>bitwise operation</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>variable scope.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve">
+For the presentation of the algorithm:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="4" tint="-0.249977111117893"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Linear search.
+Binary search.
+Big O rating. We) </t>
+    </r>
+  </si>
+  <si>
+    <t>LE 16/11/2021</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -241,6 +358,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FFFFFF00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="4" tint="-0.249977111117893"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -344,6 +467,19 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <color theme="0"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -360,19 +496,6 @@
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <color theme="0"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <alignment textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -387,10 +510,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:A1048576" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:A1048576" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
   <autoFilter ref="A1:A1048576"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="LA DATE" dataDxfId="2"/>
+    <tableColumn id="1" name="LA DATE" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleDark1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -599,8 +722,8 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -696,9 +819,19 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="11"/>
-      <c r="C7" s="9"/>
+    <row r="7" spans="1:4" ht="132" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="114.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="11"/>

</xml_diff>

<commit_message>
im sorry for pushing to late
</commit_message>
<xml_diff>
--- a/Journal De Bord YouCode 2021.xlsx
+++ b/Journal De Bord YouCode 2021.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>QU'EST-CE QU'ON A FAIS ?</t>
   </si>
@@ -417,6 +417,28 @@
   </si>
   <si>
     <t>LE 07/12/2021</t>
+  </si>
+  <si>
+    <t>Today we finished brief number 3 with the "Mobile first" Media query application.</t>
+  </si>
+  <si>
+    <t>after a brief number 4 "immovable form" was made.
+ I started with the realization of a model with Adobe xd 'Mobile and Desktop "after I coded the model with HTML and CSS.</t>
+  </si>
+  <si>
+    <t>at the end of the session I did a little documentation on the forms in Mozella MDN.</t>
+  </si>
+  <si>
+    <t>We started the session with the daylé standUp to find out about the progress of the class on the briefs and documentation,</t>
+  </si>
+  <si>
+    <t>after we made the brief number 4 a form, for the start, the realization of a mobile mockup and another desktop on the Abode xd mockup tool, and coded it with HTML and CSS, for me j I finalized brief 4, mobile and desktop part with hosting on the 000webhostapp platform "is a free hosting platform from Godaddy", at the end of the session I did a little other documentation on the flexBox concept of CSS to master the concept in a very detailed way.</t>
+  </si>
+  <si>
+    <t>LE 08/12/2021</t>
+  </si>
+  <si>
+    <t>LE 09/12/2021</t>
   </si>
 </sst>
 </file>
@@ -876,8 +898,8 @@
   </sheetPr>
   <dimension ref="A1:D1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -1121,14 +1143,29 @@
       </c>
     </row>
     <row r="18" spans="1:4" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="12"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="6"/>
+      <c r="A18" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="114.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="12"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="6"/>
+      <c r="A19" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="114.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="B20" s="8"/>

</xml_diff>